<commit_message>
together more values for spreadsheet, adding related_item functionality from the spreadsheet, updating spreadsheet with unique field names for related items
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/demo_mods.xlsx
+++ b/spec/fixtures/files/demo_mods.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26207"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nakatomi/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beekerz/Documents/cerberus/spec/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8600" yWindow="5980" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="460" windowWidth="28160" windowHeight="15940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="94">
   <si>
     <t>What is your name?</t>
   </si>
@@ -218,9 +221,6 @@
     <t>Corinne Bermon</t>
   </si>
   <si>
-    <t>neu:rx914f73k</t>
-  </si>
-  <si>
     <t>http://hdl.handle.net/2047/D20129023</t>
   </si>
   <si>
@@ -297,6 +297,18 @@
   </si>
   <si>
     <t>Governance</t>
+  </si>
+  <si>
+    <t>Original Title</t>
+  </si>
+  <si>
+    <t>Collection Title</t>
+  </si>
+  <si>
+    <t>Series Title</t>
+  </si>
+  <si>
+    <t>neu:z604pg653</t>
   </si>
 </sst>
 </file>
@@ -356,29 +368,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="none"/>
@@ -665,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BN2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -858,7 +860,7 @@
         <v>59</v>
       </c>
       <c r="BI1" s="1" t="s">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="BJ1" s="1" t="s">
         <v>60</v>
@@ -867,52 +869,52 @@
         <v>61</v>
       </c>
       <c r="BL1" s="1" t="s">
-        <v>7</v>
+        <v>91</v>
       </c>
       <c r="BM1" s="1" t="s">
         <v>62</v>
       </c>
       <c r="BN1" s="1" t="s">
-        <v>7</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -920,7 +922,7 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
@@ -935,10 +937,10 @@
       <c r="AF2" s="1"/>
       <c r="AG2" s="1"/>
       <c r="AH2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI2" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="AI2" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="AJ2" s="1">
         <v>1981</v>
@@ -952,73 +954,73 @@
         <v>1982</v>
       </c>
       <c r="AO2" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AP2" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AQ2" s="1"/>
       <c r="AR2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AS2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="AS2" s="1" t="s">
+      <c r="AT2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AT2" s="1" t="s">
+      <c r="AU2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AU2" s="1" t="s">
+      <c r="AV2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AV2" s="1" t="s">
+      <c r="AW2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AW2" s="1" t="s">
+      <c r="AX2" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="AX2" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="AY2" s="1"/>
       <c r="AZ2" s="1"/>
       <c r="BA2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB2" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="BB2" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="BC2" s="1"/>
       <c r="BD2" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="BE2" s="1"/>
       <c r="BF2" s="1"/>
       <c r="BG2" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="BH2" s="4"/>
       <c r="BI2" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="BJ2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="BK2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BL2" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="BK2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="BL2" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="BM2" s="5">
         <v>42170.508517847222</v>
       </c>
       <c r="BN2" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="BA2">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(BA2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
updating demo mods spreadsheet fixture file
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/demo_mods.xlsx
+++ b/spec/fixtures/files/demo_mods.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="141">
   <si>
     <t>What is your name?</t>
   </si>
@@ -194,9 +194,6 @@
     <t>Other notes</t>
   </si>
   <si>
-    <t>Topical Subject Headings</t>
-  </si>
-  <si>
     <t>Personal Name Subject Headings</t>
   </si>
   <si>
@@ -206,9 +203,6 @@
     <t>Corporate Name Subject Headings</t>
   </si>
   <si>
-    <t>Addiditional Corporate Name Subject Headings</t>
-  </si>
-  <si>
     <t>What is the physical location for this object?</t>
   </si>
   <si>
@@ -287,9 +281,6 @@
     <t xml:space="preserve">Donated by Citywide Educational Coalition. </t>
   </si>
   <si>
-    <t>African American students -- Massachusetts -- Boston, African Americans -- Education -- Massachusetts -- Boston, Civil rights -- Massachusetts -- Boston, Public schools -- Massachusetts -- Boston</t>
-  </si>
-  <si>
     <t>Box 1, Folder 3</t>
   </si>
   <si>
@@ -308,7 +299,157 @@
     <t>Series Title</t>
   </si>
   <si>
-    <t>neu:z604pg653</t>
+    <t>Creator 1 Role Value URI</t>
+  </si>
+  <si>
+    <t>Creator 2 Role Value URI</t>
+  </si>
+  <si>
+    <t>Creator 3 Role Value URI</t>
+  </si>
+  <si>
+    <t>Creator 4 Role Value URI</t>
+  </si>
+  <si>
+    <t>Creator 5 Role Value URI</t>
+  </si>
+  <si>
+    <t>Genre Authority</t>
+  </si>
+  <si>
+    <t>Frequency Authority</t>
+  </si>
+  <si>
+    <t>Language URI</t>
+  </si>
+  <si>
+    <t>Topical Subject Heading 1</t>
+  </si>
+  <si>
+    <t>Topical Subject Heading Authority 1</t>
+  </si>
+  <si>
+    <t>Topical Subject Heading 2</t>
+  </si>
+  <si>
+    <t>Topical Subject Heading Authority 2</t>
+  </si>
+  <si>
+    <t>Topical Subject Heading 3</t>
+  </si>
+  <si>
+    <t>Topical Subject Heading Authority 3</t>
+  </si>
+  <si>
+    <t>Topical Subject Heading 4</t>
+  </si>
+  <si>
+    <t>Topical Subject Heading Authority 4</t>
+  </si>
+  <si>
+    <t>Topical Subject Heading 5</t>
+  </si>
+  <si>
+    <t>Topical Subject Heading Authority 5</t>
+  </si>
+  <si>
+    <t>Topical Subject Heading 6</t>
+  </si>
+  <si>
+    <t>Topical Subject Heading Authority 6</t>
+  </si>
+  <si>
+    <t>Topical Subject Heading 7</t>
+  </si>
+  <si>
+    <t>Topical Subject Heading Authority 7</t>
+  </si>
+  <si>
+    <t>Additional Corporate Name Subject Headings</t>
+  </si>
+  <si>
+    <t>neu:z604w085q</t>
+  </si>
+  <si>
+    <t>http://id.loc.gov/vocabulary/relators/cre</t>
+  </si>
+  <si>
+    <t>Stannard, Marcus</t>
+  </si>
+  <si>
+    <t>personal</t>
+  </si>
+  <si>
+    <t>TREAD, Inc.</t>
+  </si>
+  <si>
+    <t>aat</t>
+  </si>
+  <si>
+    <t>marcfrequency</t>
+  </si>
+  <si>
+    <t>http://id.loc.gov/vocabulary/iso639-2/eng</t>
+  </si>
+  <si>
+    <t>African American students -- Massachusetts -- Boston</t>
+  </si>
+  <si>
+    <t>lcsh</t>
+  </si>
+  <si>
+    <t>African Americans -- Education -- Massachusetts -- Boston</t>
+  </si>
+  <si>
+    <t>Civil rights -- Massachusetts -- Boston</t>
+  </si>
+  <si>
+    <t>Public schools -- Massachusetts -- Boston</t>
+  </si>
+  <si>
+    <t>neu:z604w088j</t>
+  </si>
+  <si>
+    <t>http://hdl.handle.net/2047/D20194578</t>
+  </si>
+  <si>
+    <t>M130.B05.F020.001.pdf</t>
+  </si>
+  <si>
+    <t>M130.B05.F020.001</t>
+  </si>
+  <si>
+    <t>Citywide Educational Coalition project budget summary, September 1, 1978 - August 31, 1979.</t>
+  </si>
+  <si>
+    <t>records (documents)</t>
+  </si>
+  <si>
+    <t>1978-09-01</t>
+  </si>
+  <si>
+    <t>approximate</t>
+  </si>
+  <si>
+    <t>7 pages</t>
+  </si>
+  <si>
+    <t>Contains budget information for CWEC for school year 1978-1979.</t>
+  </si>
+  <si>
+    <t>Busing for school integration -- Massachusetts -- Boston</t>
+  </si>
+  <si>
+    <t>School integration -- Massachusetts -- Boston</t>
+  </si>
+  <si>
+    <t>Garrity, W. Arthur (Wendell Arthur), 1920-1999; Smith, Mary Ellen</t>
+  </si>
+  <si>
+    <t>Box 5, Folder 20</t>
+  </si>
+  <si>
+    <t>Executive Staff</t>
   </si>
 </sst>
 </file>
@@ -318,7 +459,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -340,6 +481,19 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -365,10 +519,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -376,11 +531,42 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none"/>
@@ -665,10 +851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BN2"/>
+  <dimension ref="A1:CI3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -678,7 +864,7 @@
     <col min="3" max="3" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -725,207 +911,282 @@
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AL1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AP1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="BA1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="BF1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="BY1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="CA1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="CB1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="CC1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="CD1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="CE1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="CF1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="CG1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="CH1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="CI1" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:87" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BL1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM1" s="1" t="s">
+      <c r="B2" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="BN1" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="V2" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="W2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
@@ -936,96 +1197,316 @@
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
       <c r="AG2" s="1"/>
-      <c r="AH2" s="1" t="s">
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="1"/>
+      <c r="AM2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AP2" s="1">
+        <v>1981</v>
+      </c>
+      <c r="AQ2" s="1">
+        <v>1982</v>
+      </c>
+      <c r="AR2" s="1"/>
+      <c r="AS2" s="1"/>
+      <c r="AT2" s="1">
+        <v>1982</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AV2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AW2" s="1"/>
+      <c r="AX2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AJ2" s="1">
-        <v>1981</v>
-      </c>
-      <c r="AK2" s="1">
-        <v>1982</v>
-      </c>
-      <c r="AL2" s="1"/>
-      <c r="AM2" s="1"/>
-      <c r="AN2" s="1">
-        <v>1982</v>
-      </c>
-      <c r="AO2" s="1" t="s">
+      <c r="AY2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AZ2" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="BA2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="BB2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BC2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BD2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BE2" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="BF2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BG2" s="1"/>
+      <c r="BH2" s="1"/>
+      <c r="BI2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="BJ2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BK2" s="1"/>
+      <c r="BL2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="BM2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="BN2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="BO2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="BP2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="BQ2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="BR2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="BS2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="BT2" s="1"/>
+      <c r="BU2" s="1"/>
+      <c r="BV2" s="1"/>
+      <c r="BW2" s="1"/>
+      <c r="BX2" s="1"/>
+      <c r="BY2" s="1"/>
+      <c r="BZ2" s="1"/>
+      <c r="CA2" s="1"/>
+      <c r="CB2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="CC2" s="4"/>
+      <c r="CD2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="CE2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="CF2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="CG2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="CH2" s="5">
+        <v>42170.508517847222</v>
+      </c>
+      <c r="CI2" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:87" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="10"/>
+      <c r="H3" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="O3" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="AP2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AQ2" s="1"/>
-      <c r="AR2" s="1" t="s">
+      <c r="P3" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="10"/>
+      <c r="AC3" s="10"/>
+      <c r="AD3" s="10"/>
+      <c r="AE3" s="10"/>
+      <c r="AF3" s="10"/>
+      <c r="AG3" s="10"/>
+      <c r="AH3" s="10"/>
+      <c r="AI3" s="10"/>
+      <c r="AJ3" s="10"/>
+      <c r="AK3" s="10"/>
+      <c r="AL3" s="10"/>
+      <c r="AM3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN3" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="AO3" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="AP3" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="AQ3" s="10"/>
+      <c r="AR3" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="AS3" s="10"/>
+      <c r="AT3" s="10"/>
+      <c r="AU3" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AV3" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="AW3" s="10"/>
+      <c r="AX3" s="10"/>
+      <c r="AY3" s="10"/>
+      <c r="AZ3" s="10"/>
+      <c r="BA3" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="AS2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AT2" s="1" t="s">
+      <c r="BB3" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="BC3" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="AU2" s="1" t="s">
+      <c r="BD3" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="AV2" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AW2" s="1" t="s">
+      <c r="BE3" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="BF3" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="BG3" s="10"/>
+      <c r="BH3" s="10"/>
+      <c r="BI3" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="AX2" s="1" t="s">
+      <c r="BJ3" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="AY2" s="1"/>
-      <c r="AZ2" s="1"/>
-      <c r="BA2" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="BB2" s="1" t="s">
+      <c r="BK3" s="10"/>
+      <c r="BL3" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="BM3" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="BN3" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="BO3" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="BP3" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="BQ3" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="BR3" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="BS3" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="BT3" s="8"/>
+      <c r="BU3" s="8"/>
+      <c r="BV3" s="8"/>
+      <c r="BW3" s="8"/>
+      <c r="BX3" s="8"/>
+      <c r="BY3" s="8"/>
+      <c r="BZ3" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="CA3" s="10"/>
+      <c r="CB3" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="CC3" s="13"/>
+      <c r="CD3" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="CE3" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="CF3" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="CG3" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="BC2" s="1"/>
-      <c r="BD2" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="BE2" s="1"/>
-      <c r="BF2" s="1"/>
-      <c r="BG2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="BH2" s="4"/>
-      <c r="BI2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BJ2" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="BK2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="BL2" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="BM2" s="5">
-        <v>42170.508517847222</v>
-      </c>
-      <c r="BN2" s="1" t="s">
-        <v>89</v>
+      <c r="CH3" s="14">
+        <v>42243.733247824071</v>
+      </c>
+      <c r="CI3" s="8" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="BA2">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(BA2))&gt;0</formula>
+  <conditionalFormatting sqref="BI2">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
+      <formula>LEN(TRIM(BI2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="P2" r:id="rId3"/>
+    <hyperlink ref="P3" r:id="rId4"/>
+    <hyperlink ref="U2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updating fixture file with more complex examples and creator authority
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/demo_mods.xlsx
+++ b/spec/fixtures/files/demo_mods.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="149">
   <si>
     <t>What is your name?</t>
   </si>
@@ -374,9 +374,6 @@
     <t>http://id.loc.gov/vocabulary/relators/cre</t>
   </si>
   <si>
-    <t>Stannard, Marcus</t>
-  </si>
-  <si>
     <t>personal</t>
   </si>
   <si>
@@ -450,6 +447,33 @@
   </si>
   <si>
     <t>Executive Staff</t>
+  </si>
+  <si>
+    <t>Citywide Educational Coalition | URI for value</t>
+  </si>
+  <si>
+    <t>Creator 1 Authority</t>
+  </si>
+  <si>
+    <t>lcsh | lcsh URI</t>
+  </si>
+  <si>
+    <t>Creator 2 Authority</t>
+  </si>
+  <si>
+    <t>Stannard | Marcus | | | URI for Stannard</t>
+  </si>
+  <si>
+    <t>Creator 3 Authority</t>
+  </si>
+  <si>
+    <t>Creator 4 Authority</t>
+  </si>
+  <si>
+    <t>Creator 5 Authority</t>
+  </si>
+  <si>
+    <t>Garrity | W. Arthur (Wendell Arthur)| Rev| 1920-1999 | URI for value</t>
   </si>
 </sst>
 </file>
@@ -544,29 +568,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="none"/>
@@ -851,10 +853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CI3"/>
+  <dimension ref="A1:CN3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -864,7 +866,7 @@
     <col min="3" max="3" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:87" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:92" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -905,229 +907,244 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AH1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AN1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BW1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BX1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="CA1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="CB1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="CC1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="CD1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="CE1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="CA1" s="1" t="s">
+      <c r="CF1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="CB1" s="1" t="s">
+      <c r="CG1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="CC1" s="1" t="s">
+      <c r="CH1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="CD1" s="1" t="s">
+      <c r="CI1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="CE1" s="1" t="s">
+      <c r="CJ1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="CF1" s="1" t="s">
+      <c r="CK1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="CG1" s="1" t="s">
+      <c r="CL1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="CH1" s="1" t="s">
+      <c r="CM1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="CI1" s="1" t="s">
+      <c r="CN1" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:87" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:92" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>61</v>
       </c>
@@ -1157,38 +1174,42 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
-        <v>68</v>
+        <v>140</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="Q2" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="8" t="s">
+      <c r="R2" s="1"/>
+      <c r="S2" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="U2" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="V2" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="X2" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="T2" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="U2" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="V2" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="W2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
@@ -1202,174 +1223,187 @@
       <c r="AJ2" s="1"/>
       <c r="AK2" s="1"/>
       <c r="AL2" s="1"/>
-      <c r="AM2" s="1" t="s">
+      <c r="AM2" s="1"/>
+      <c r="AN2" s="1"/>
+      <c r="AO2" s="1"/>
+      <c r="AP2" s="1"/>
+      <c r="AQ2" s="1"/>
+      <c r="AR2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AN2" s="1" t="s">
+      <c r="AS2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AT2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AU2" s="1">
+        <v>1981</v>
+      </c>
+      <c r="AV2" s="1">
+        <v>1982</v>
+      </c>
+      <c r="AW2" s="1"/>
+      <c r="AX2" s="1"/>
+      <c r="AY2" s="1">
+        <v>1982</v>
+      </c>
+      <c r="AZ2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BA2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BB2" s="1"/>
+      <c r="BC2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BE2" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="AP2" s="1">
-        <v>1981</v>
-      </c>
-      <c r="AQ2" s="1">
-        <v>1982</v>
-      </c>
-      <c r="AR2" s="1"/>
-      <c r="AS2" s="1"/>
-      <c r="AT2" s="1">
-        <v>1982</v>
-      </c>
-      <c r="AU2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AV2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AW2" s="1"/>
-      <c r="AX2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AY2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AZ2" s="9" t="s">
+      <c r="BF2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="BG2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BH2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BI2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BJ2" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="BA2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="BB2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="BC2" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="BD2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="BE2" s="1" t="s">
+      <c r="BK2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BL2" s="1"/>
+      <c r="BM2" s="1"/>
+      <c r="BN2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="BO2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BP2" s="1"/>
+      <c r="BQ2" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="BF2" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="BG2" s="1"/>
-      <c r="BH2" s="1"/>
-      <c r="BI2" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="BJ2" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="BK2" s="1"/>
-      <c r="BL2" s="1" t="s">
+      <c r="BR2" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="BM2" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="BN2" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="BO2" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="BP2" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="BQ2" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="BR2" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="BS2" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="BT2" s="1"/>
-      <c r="BU2" s="1"/>
-      <c r="BV2" s="1"/>
-      <c r="BW2" s="1"/>
-      <c r="BX2" s="1"/>
+      <c r="BT2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="BU2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="BV2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="BW2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="BX2" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="BY2" s="1"/>
       <c r="BZ2" s="1"/>
       <c r="CA2" s="1"/>
-      <c r="CB2" s="3" t="s">
+      <c r="CB2" s="1"/>
+      <c r="CC2" s="1"/>
+      <c r="CD2" s="1"/>
+      <c r="CE2" s="1"/>
+      <c r="CF2" s="1"/>
+      <c r="CG2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="CC2" s="4"/>
-      <c r="CD2" s="1" t="s">
+      <c r="CH2" s="4"/>
+      <c r="CI2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="CE2" s="1" t="s">
+      <c r="CJ2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="CF2" s="1" t="s">
+      <c r="CK2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="CG2" s="1" t="s">
+      <c r="CL2" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="CH2" s="5">
+      <c r="CM2" s="5">
         <v>42170.508517847222</v>
       </c>
-      <c r="CI2" s="1" t="s">
+      <c r="CN2" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:87" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:92" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>61</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="D3" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>129</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>65</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
       <c r="M3" s="8" t="s">
-        <v>68</v>
+        <v>140</v>
       </c>
       <c r="N3" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="O3" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="P3" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="Q3" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="Q3" s="10"/>
       <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
+      <c r="S3" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="T3" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="U3" s="10" t="s">
+        <v>115</v>
+      </c>
       <c r="V3" s="10"/>
-      <c r="W3" s="8" t="s">
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="10"/>
       <c r="Z3" s="10"/>
       <c r="AA3" s="10"/>
       <c r="AB3" s="10"/>
@@ -1383,131 +1417,137 @@
       <c r="AJ3" s="10"/>
       <c r="AK3" s="10"/>
       <c r="AL3" s="10"/>
-      <c r="AM3" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="AN3" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="AO3" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="AP3" s="8" t="s">
-        <v>132</v>
-      </c>
+      <c r="AM3" s="10"/>
+      <c r="AN3" s="10"/>
+      <c r="AO3" s="10"/>
+      <c r="AP3" s="10"/>
       <c r="AQ3" s="10"/>
       <c r="AR3" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="AS3" s="10"/>
-      <c r="AT3" s="10"/>
+        <v>72</v>
+      </c>
+      <c r="AS3" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="AT3" s="12" t="s">
+        <v>117</v>
+      </c>
       <c r="AU3" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="AV3" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="AW3" s="10"/>
+        <v>131</v>
+      </c>
+      <c r="AV3" s="10"/>
+      <c r="AW3" s="8" t="s">
+        <v>132</v>
+      </c>
       <c r="AX3" s="10"/>
       <c r="AY3" s="10"/>
-      <c r="AZ3" s="10"/>
+      <c r="AZ3" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="BA3" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="BB3" s="10"/>
+      <c r="BC3" s="10"/>
+      <c r="BD3" s="10"/>
+      <c r="BE3" s="10"/>
+      <c r="BF3" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="BB3" s="8" t="s">
+      <c r="BG3" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="BH3" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="BI3" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="BJ3" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="BK3" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="BC3" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="BD3" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="BE3" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="BF3" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="BG3" s="10"/>
-      <c r="BH3" s="10"/>
-      <c r="BI3" s="8" t="s">
+      <c r="BL3" s="10"/>
+      <c r="BM3" s="10"/>
+      <c r="BN3" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="BJ3" s="8" t="s">
+      <c r="BO3" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="BK3" s="10"/>
-      <c r="BL3" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="BM3" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="BN3" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="BO3" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="BP3" s="8" t="s">
-        <v>125</v>
-      </c>
+      <c r="BP3" s="10"/>
       <c r="BQ3" s="8" t="s">
         <v>122</v>
       </c>
       <c r="BR3" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="BS3" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="BT3" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="BU3" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="BV3" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="BW3" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="BX3" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="BY3" s="8"/>
+      <c r="BZ3" s="8"/>
+      <c r="CA3" s="8"/>
+      <c r="CB3" s="8"/>
+      <c r="CC3" s="8"/>
+      <c r="CD3" s="8"/>
+      <c r="CE3" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="BS3" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="BT3" s="8"/>
-      <c r="BU3" s="8"/>
-      <c r="BV3" s="8"/>
-      <c r="BW3" s="8"/>
-      <c r="BX3" s="8"/>
-      <c r="BY3" s="8"/>
-      <c r="BZ3" s="8" t="s">
+      <c r="CF3" s="10"/>
+      <c r="CG3" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="CH3" s="13"/>
+      <c r="CI3" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="CJ3" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="CA3" s="10"/>
-      <c r="CB3" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="CC3" s="13"/>
-      <c r="CD3" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="CE3" s="8" t="s">
+      <c r="CK3" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="CL3" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="CM3" s="14">
+        <v>42243.733247824071</v>
+      </c>
+      <c r="CN3" s="8" t="s">
         <v>139</v>
-      </c>
-      <c r="CF3" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="CG3" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="CH3" s="14">
-        <v>42243.733247824071</v>
-      </c>
-      <c r="CI3" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="BI2">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
-      <formula>LEN(TRIM(BI2))&gt;0</formula>
+  <conditionalFormatting sqref="BN2">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(BN2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="P2" r:id="rId3"/>
-    <hyperlink ref="P3" r:id="rId4"/>
-    <hyperlink ref="U2" r:id="rId5"/>
+    <hyperlink ref="Q2" r:id="rId3"/>
+    <hyperlink ref="Q3" r:id="rId4"/>
+    <hyperlink ref="W2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactor fields with multiples to accomodate n fields instead of a limited number, applying name subjects correctly in mods, adding more validity checks and core file health checks, changing handle mismatch to be a yellow/modified state
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/demo_mods.xlsx
+++ b/spec/fixtures/files/demo_mods.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="159">
   <si>
     <t>What is your name?</t>
   </si>
@@ -194,15 +194,6 @@
     <t>Other notes</t>
   </si>
   <si>
-    <t>Personal Name Subject Headings</t>
-  </si>
-  <si>
-    <t>Additional Personal Name Subject Headings</t>
-  </si>
-  <si>
-    <t>Corporate Name Subject Headings</t>
-  </si>
-  <si>
     <t>What is the physical location for this object?</t>
   </si>
   <si>
@@ -365,9 +356,6 @@
     <t>Topical Subject Heading Authority 7</t>
   </si>
   <si>
-    <t>Additional Corporate Name Subject Headings</t>
-  </si>
-  <si>
     <t>neu:z604w085q</t>
   </si>
   <si>
@@ -440,9 +428,6 @@
     <t>School integration -- Massachusetts -- Boston</t>
   </si>
   <si>
-    <t>Garrity, W. Arthur (Wendell Arthur), 1920-1999; Smith, Mary Ellen</t>
-  </si>
-  <si>
     <t>Box 5, Folder 20</t>
   </si>
   <si>
@@ -474,16 +459,62 @@
   </si>
   <si>
     <t>Garrity | W. Arthur (Wendell Arthur)| Rev| 1920-1999 | URI for value</t>
+  </si>
+  <si>
+    <t>http://hdl.handle.net/2047/D20129027</t>
+  </si>
+  <si>
+    <t>neu:z604w088f90asadj</t>
+  </si>
+  <si>
+    <t>neu:z604qj33d</t>
+  </si>
+  <si>
+    <t>neu:z604pm73m</t>
+  </si>
+  <si>
+    <t>Subject Name 1</t>
+  </si>
+  <si>
+    <t>Subject Name 1 Authority</t>
+  </si>
+  <si>
+    <t>Subject Name 1 Name Type</t>
+  </si>
+  <si>
+    <t>Subject Name 1 Affiliation</t>
+  </si>
+  <si>
+    <t>Garrity | W. Arthur (Wendell Arthur) | | 1920-1999 | Value URI</t>
+  </si>
+  <si>
+    <t>Smith | Mary Ellen ||| Value URI</t>
+  </si>
+  <si>
+    <t>Subject Name 2</t>
+  </si>
+  <si>
+    <t>Subject Name 2 Authority</t>
+  </si>
+  <si>
+    <t>Subject Name 2 Name Type</t>
+  </si>
+  <si>
+    <t>Subject Name 2 Affiliation</t>
+  </si>
+  <si>
+    <t>http://hdl.handle.net/2047/D10000740</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -494,17 +525,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <u/>
@@ -520,18 +540,12 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -545,24 +559,21 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -853,28 +864,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CN3"/>
+  <dimension ref="A1:CR7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3"/>
+    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" zoomScalePageLayoutView="127" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.5" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" customWidth="1"/>
-    <col min="3" max="3" width="34" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="72.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="51.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="51" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="19" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="9" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="8" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="104.83203125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="102" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="34" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="28" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="28" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="28" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="28" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="28" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="28" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="28" bestFit="1" customWidth="1"/>
+    <col min="83" max="87" width="28" customWidth="1"/>
+    <col min="88" max="88" width="50.5" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="72.5" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="34" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="35.83203125" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:92" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -907,7 +1007,7 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>13</v>
@@ -916,7 +1016,7 @@
         <v>14</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>15</v>
@@ -925,7 +1025,7 @@
         <v>16</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>17</v>
@@ -934,7 +1034,7 @@
         <v>18</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>19</v>
@@ -946,7 +1046,7 @@
         <v>21</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>22</v>
@@ -955,7 +1055,7 @@
         <v>23</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>24</v>
@@ -964,7 +1064,7 @@
         <v>25</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="AH1" s="1" t="s">
         <v>26</v>
@@ -973,7 +1073,7 @@
         <v>27</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>28</v>
@@ -982,7 +1082,7 @@
         <v>29</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="AN1" s="1" t="s">
         <v>30</v>
@@ -991,7 +1091,7 @@
         <v>31</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="AQ1" s="1" t="s">
         <v>32</v>
@@ -1003,7 +1103,7 @@
         <v>34</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AU1" s="1" t="s">
         <v>35</v>
@@ -1036,7 +1136,7 @@
         <v>44</v>
       </c>
       <c r="BE1" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="BF1" s="1" t="s">
         <v>45</v>
@@ -1051,7 +1151,7 @@
         <v>48</v>
       </c>
       <c r="BJ1" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="BK1" s="1" t="s">
         <v>49</v>
@@ -1072,143 +1172,155 @@
         <v>54</v>
       </c>
       <c r="BQ1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="BT1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BW1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="BX1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="CA1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="CB1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="CC1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="CA1" s="1" t="s">
+      <c r="CD1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="CB1" s="1" t="s">
+      <c r="CE1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="CF1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="CG1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="CH1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="CI1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="CJ1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="CK1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="CL1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="CM1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="CN1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="CO1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="CP1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="CQ1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="CR1" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:96" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="CC1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="CD1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="CE1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="CF1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="CG1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="CH1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="CI1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="CJ1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="CK1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="CL1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="CM1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="CN1" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:92" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>114</v>
+        <v>67</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>110</v>
       </c>
       <c r="R2" s="1"/>
-      <c r="S2" s="8" t="s">
-        <v>144</v>
+      <c r="S2" s="6" t="s">
+        <v>139</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="U2" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="V2" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="W2" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>116</v>
+        <v>137</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>112</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
@@ -1229,13 +1341,13 @@
       <c r="AP2" s="1"/>
       <c r="AQ2" s="1"/>
       <c r="AR2" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="AS2" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="AT2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="AU2" s="1">
         <v>1981</v>
@@ -1249,71 +1361,71 @@
         <v>1982</v>
       </c>
       <c r="AZ2" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="BA2" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="BB2" s="1"/>
       <c r="BC2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BD2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BE2" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="BF2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BG2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BD2" s="1" t="s">
+      <c r="BH2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="BE2" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="BF2" s="1" t="s">
+      <c r="BI2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="BG2" s="1" t="s">
+      <c r="BJ2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="BK2" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="BH2" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="BI2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="BJ2" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="BK2" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="BL2" s="1"/>
       <c r="BM2" s="1"/>
       <c r="BN2" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="BO2" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="BP2" s="1"/>
       <c r="BQ2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="BR2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="BS2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="BT2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="BU2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="BV2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="BW2" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="BR2" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="BS2" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="BT2" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="BU2" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="BV2" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="BW2" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="BX2" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="BY2" s="1"/>
       <c r="BZ2" s="1"/>
@@ -1321,217 +1433,981 @@
       <c r="CB2" s="1"/>
       <c r="CC2" s="1"/>
       <c r="CD2" s="1"/>
-      <c r="CE2" s="1"/>
-      <c r="CF2" s="1"/>
-      <c r="CG2" s="3" t="s">
+      <c r="CE2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="CF2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="CG2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="CH2" s="1"/>
+      <c r="CI2" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="CJ2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="CK2" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="CL2" s="2"/>
+      <c r="CM2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="CN2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="CO2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="CP2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="CQ2" s="3">
+        <v>42170.508518518516</v>
+      </c>
+      <c r="CR2" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:96" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="U3" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="CH2" s="4"/>
-      <c r="CI2" s="1" t="s">
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="8"/>
+      <c r="AE3" s="8"/>
+      <c r="AF3" s="8"/>
+      <c r="AG3" s="8"/>
+      <c r="AH3" s="8"/>
+      <c r="AI3" s="8"/>
+      <c r="AJ3" s="8"/>
+      <c r="AK3" s="8"/>
+      <c r="AL3" s="8"/>
+      <c r="AM3" s="8"/>
+      <c r="AN3" s="8"/>
+      <c r="AO3" s="8"/>
+      <c r="AP3" s="8"/>
+      <c r="AQ3" s="8"/>
+      <c r="AR3" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="AS3" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="AT3" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="AU3" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="AV3" s="8"/>
+      <c r="AW3" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="AX3" s="8"/>
+      <c r="AY3" s="8"/>
+      <c r="AZ3" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="BA3" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="BB3" s="8"/>
+      <c r="BC3" s="8"/>
+      <c r="BD3" s="8"/>
+      <c r="BE3" s="8"/>
+      <c r="BF3" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="BG3" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="BH3" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="BI3" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="BJ3" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="BK3" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="BL3" s="8"/>
+      <c r="BM3" s="8"/>
+      <c r="BN3" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="BO3" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="BP3" s="8"/>
+      <c r="BQ3" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="BR3" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="BS3" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="BT3" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="BU3" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="BV3" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="BW3" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="BX3" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="BY3" s="6"/>
+      <c r="BZ3" s="6"/>
+      <c r="CA3" s="6"/>
+      <c r="CB3" s="6"/>
+      <c r="CC3" s="6"/>
+      <c r="CD3" s="6"/>
+      <c r="CE3" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="CF3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="CG3" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="CH3" s="6"/>
+      <c r="CI3" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="CJ3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="CK3" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="CL3" s="9"/>
+      <c r="CM3" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="CN3" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="CO3" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="CP3" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="CQ3" s="10">
+        <v>42243.733247824071</v>
+      </c>
+      <c r="CR3" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:96" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="P4" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="CJ2" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="CK2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="CL2" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="CM2" s="5">
-        <v>42170.508517847222</v>
-      </c>
-      <c r="CN2" s="1" t="s">
-        <v>86</v>
+      <c r="Q4" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="T4" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="U4" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+      <c r="AC4" s="8"/>
+      <c r="AD4" s="8"/>
+      <c r="AE4" s="8"/>
+      <c r="AF4" s="8"/>
+      <c r="AG4" s="8"/>
+      <c r="AH4" s="8"/>
+      <c r="AI4" s="8"/>
+      <c r="AJ4" s="8"/>
+      <c r="AK4" s="8"/>
+      <c r="AL4" s="8"/>
+      <c r="AM4" s="8"/>
+      <c r="AN4" s="8"/>
+      <c r="AO4" s="8"/>
+      <c r="AP4" s="8"/>
+      <c r="AQ4" s="8"/>
+      <c r="AR4" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="AS4" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="AT4" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="AU4" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="AV4" s="8"/>
+      <c r="AW4" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="AX4" s="8"/>
+      <c r="AY4" s="8"/>
+      <c r="AZ4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="BA4" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="BB4" s="8"/>
+      <c r="BC4" s="8"/>
+      <c r="BD4" s="8"/>
+      <c r="BE4" s="8"/>
+      <c r="BF4" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="BG4" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="BH4" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="BI4" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="BJ4" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="BK4" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="BL4" s="8"/>
+      <c r="BM4" s="8"/>
+      <c r="BN4" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="BO4" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="BP4" s="8"/>
+      <c r="BQ4" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="BR4" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="BS4" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="BT4" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="BU4" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="BV4" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="BW4" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="BX4" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="BY4" s="6"/>
+      <c r="BZ4" s="6"/>
+      <c r="CA4" s="6"/>
+      <c r="CB4" s="6"/>
+      <c r="CC4" s="6"/>
+      <c r="CD4" s="6"/>
+      <c r="CE4" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="CF4" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="CG4" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="CH4" s="6"/>
+      <c r="CI4" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="CJ4" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="CK4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="CL4" s="9"/>
+      <c r="CM4" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="CN4" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="CO4" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="CP4" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="CQ4" s="10">
+        <v>42243.733247824071</v>
+      </c>
+      <c r="CR4" s="6" t="s">
+        <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:92" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" s="10" t="s">
+    <row r="5" spans="1:96" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="T5" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="U5" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+      <c r="AC5" s="8"/>
+      <c r="AD5" s="8"/>
+      <c r="AE5" s="8"/>
+      <c r="AF5" s="8"/>
+      <c r="AG5" s="8"/>
+      <c r="AH5" s="8"/>
+      <c r="AI5" s="8"/>
+      <c r="AJ5" s="8"/>
+      <c r="AK5" s="8"/>
+      <c r="AL5" s="8"/>
+      <c r="AM5" s="8"/>
+      <c r="AN5" s="8"/>
+      <c r="AO5" s="8"/>
+      <c r="AP5" s="8"/>
+      <c r="AQ5" s="8"/>
+      <c r="AR5" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="AS5" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="AT5" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="AU5" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="AV5" s="8"/>
+      <c r="AW5" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="AX5" s="8"/>
+      <c r="AY5" s="8"/>
+      <c r="AZ5" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="BA5" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="BB5" s="8"/>
+      <c r="BC5" s="8"/>
+      <c r="BD5" s="8"/>
+      <c r="BE5" s="8"/>
+      <c r="BF5" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="BG5" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="BH5" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="BI5" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="BJ5" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="BK5" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="BL5" s="8"/>
+      <c r="BM5" s="8"/>
+      <c r="BN5" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="BO5" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="BP5" s="8"/>
+      <c r="BQ5" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="BR5" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="BS5" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="BT5" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="BU5" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="BV5" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="BW5" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="BX5" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="BY5" s="6"/>
+      <c r="BZ5" s="6"/>
+      <c r="CA5" s="6"/>
+      <c r="CB5" s="6"/>
+      <c r="CC5" s="6"/>
+      <c r="CD5" s="6"/>
+      <c r="CE5" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="CF5" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="CG5" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="CH5" s="6"/>
+      <c r="CI5" s="6"/>
+      <c r="CJ5" s="6"/>
+      <c r="CK5" s="8"/>
+      <c r="CL5" s="9"/>
+      <c r="CM5" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="CN5" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="CO5" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="CP5" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="CQ5" s="3">
+        <v>42170.508518518516</v>
+      </c>
+      <c r="CR5" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:96" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="T6" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="U6" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z6" s="8"/>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="8"/>
+      <c r="AC6" s="8"/>
+      <c r="AD6" s="8"/>
+      <c r="AE6" s="8"/>
+      <c r="AF6" s="8"/>
+      <c r="AG6" s="8"/>
+      <c r="AH6" s="8"/>
+      <c r="AI6" s="8"/>
+      <c r="AJ6" s="8"/>
+      <c r="AK6" s="8"/>
+      <c r="AL6" s="8"/>
+      <c r="AM6" s="8"/>
+      <c r="AN6" s="8"/>
+      <c r="AO6" s="8"/>
+      <c r="AP6" s="8"/>
+      <c r="AQ6" s="8"/>
+      <c r="AR6" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="AS6" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="AT6" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="AU6" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="AV6" s="8"/>
+      <c r="AW6" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="AX6" s="8"/>
+      <c r="AY6" s="8"/>
+      <c r="AZ6" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="8" t="s">
+      <c r="BA6" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="BB6" s="8"/>
+      <c r="BC6" s="8"/>
+      <c r="BD6" s="8"/>
+      <c r="BE6" s="8"/>
+      <c r="BF6" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="BG6" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="O3" s="8" t="s">
+      <c r="BH6" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="BI6" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="BJ6" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="BK6" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="BL6" s="8"/>
+      <c r="BM6" s="8"/>
+      <c r="BN6" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="BO6" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="BP6" s="8"/>
+      <c r="BQ6" s="6"/>
+      <c r="BR6" s="6"/>
+      <c r="BS6" s="6"/>
+      <c r="BT6" s="6"/>
+      <c r="BU6" s="6"/>
+      <c r="BV6" s="6"/>
+      <c r="BW6" s="6"/>
+      <c r="BX6" s="6"/>
+      <c r="BY6" s="6"/>
+      <c r="BZ6" s="6"/>
+      <c r="CA6" s="6"/>
+      <c r="CB6" s="6"/>
+      <c r="CC6" s="6"/>
+      <c r="CD6" s="6"/>
+      <c r="CE6" s="6"/>
+      <c r="CF6" s="6"/>
+      <c r="CG6" s="6"/>
+      <c r="CH6" s="6"/>
+      <c r="CI6" s="6"/>
+      <c r="CJ6" s="6"/>
+      <c r="CK6" s="8"/>
+      <c r="CL6" s="9"/>
+      <c r="CM6" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="CN6" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="CO6" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="CP6" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="CQ6" s="11">
+        <v>42243.733247824071</v>
+      </c>
+      <c r="CR6" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:96" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="T7" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="U7" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z7" s="8"/>
+      <c r="AA7" s="8"/>
+      <c r="AB7" s="8"/>
+      <c r="AC7" s="8"/>
+      <c r="AD7" s="8"/>
+      <c r="AE7" s="8"/>
+      <c r="AF7" s="8"/>
+      <c r="AG7" s="8"/>
+      <c r="AH7" s="8"/>
+      <c r="AI7" s="8"/>
+      <c r="AJ7" s="8"/>
+      <c r="AK7" s="8"/>
+      <c r="AL7" s="8"/>
+      <c r="AM7" s="8"/>
+      <c r="AN7" s="8"/>
+      <c r="AO7" s="8"/>
+      <c r="AP7" s="8"/>
+      <c r="AQ7" s="8"/>
+      <c r="AR7" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="P3" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="T3" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="U3" s="10" t="s">
+      <c r="AS7" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="AT7" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="AU7" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="AV7" s="8"/>
+      <c r="AW7" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="AX7" s="8"/>
+      <c r="AY7" s="8"/>
+      <c r="AZ7" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="BA7" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="BB7" s="8"/>
+      <c r="BC7" s="8"/>
+      <c r="BD7" s="8"/>
+      <c r="BE7" s="8"/>
+      <c r="BF7" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="BG7" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="BH7" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="BI7" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="BJ7" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="V3" s="10"/>
-      <c r="W3" s="10"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="Z3" s="10"/>
-      <c r="AA3" s="10"/>
-      <c r="AB3" s="10"/>
-      <c r="AC3" s="10"/>
-      <c r="AD3" s="10"/>
-      <c r="AE3" s="10"/>
-      <c r="AF3" s="10"/>
-      <c r="AG3" s="10"/>
-      <c r="AH3" s="10"/>
-      <c r="AI3" s="10"/>
-      <c r="AJ3" s="10"/>
-      <c r="AK3" s="10"/>
-      <c r="AL3" s="10"/>
-      <c r="AM3" s="10"/>
-      <c r="AN3" s="10"/>
-      <c r="AO3" s="10"/>
-      <c r="AP3" s="10"/>
-      <c r="AQ3" s="10"/>
-      <c r="AR3" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="AS3" s="8" t="s">
+      <c r="BK7" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="AT3" s="12" t="s">
+      <c r="BL7" s="8"/>
+      <c r="BM7" s="8"/>
+      <c r="BN7" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="BO7" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="BP7" s="8"/>
+      <c r="BQ7" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="BR7" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="AU3" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="AV3" s="10"/>
-      <c r="AW3" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="AX3" s="10"/>
-      <c r="AY3" s="10"/>
-      <c r="AZ3" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="BA3" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="BB3" s="10"/>
-      <c r="BC3" s="10"/>
-      <c r="BD3" s="10"/>
-      <c r="BE3" s="10"/>
-      <c r="BF3" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="BG3" s="8" t="s">
+      <c r="BS7" s="6"/>
+      <c r="BT7" s="6"/>
+      <c r="BU7" s="6"/>
+      <c r="BV7" s="6"/>
+      <c r="BW7" s="6"/>
+      <c r="BX7" s="6"/>
+      <c r="BY7" s="6"/>
+      <c r="BZ7" s="6"/>
+      <c r="CA7" s="6"/>
+      <c r="CB7" s="6"/>
+      <c r="CC7" s="6"/>
+      <c r="CD7" s="6"/>
+      <c r="CE7" s="6"/>
+      <c r="CF7" s="6"/>
+      <c r="CG7" s="6"/>
+      <c r="CH7" s="6"/>
+      <c r="CI7" s="6"/>
+      <c r="CJ7" s="6"/>
+      <c r="CK7" s="8"/>
+      <c r="CL7" s="9"/>
+      <c r="CM7" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="CN7" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="BH3" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="BI3" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="BJ3" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="BK3" s="8" t="s">
+      <c r="CO7" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="CP7" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="CQ7" s="11">
+        <v>42243.733247824071</v>
+      </c>
+      <c r="CR7" s="6" t="s">
         <v>134</v>
-      </c>
-      <c r="BL3" s="10"/>
-      <c r="BM3" s="10"/>
-      <c r="BN3" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="BO3" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="BP3" s="10"/>
-      <c r="BQ3" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="BR3" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="BS3" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="BT3" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="BU3" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="BV3" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="BW3" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="BX3" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="BY3" s="8"/>
-      <c r="BZ3" s="8"/>
-      <c r="CA3" s="8"/>
-      <c r="CB3" s="8"/>
-      <c r="CC3" s="8"/>
-      <c r="CD3" s="8"/>
-      <c r="CE3" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="CF3" s="10"/>
-      <c r="CG3" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="CH3" s="13"/>
-      <c r="CI3" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="CJ3" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="CK3" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="CL3" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="CM3" s="14">
-        <v>42243.733247824071</v>
-      </c>
-      <c r="CN3" s="8" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1541,11 +2417,18 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="Q2" r:id="rId3"/>
-    <hyperlink ref="Q3" r:id="rId4"/>
-    <hyperlink ref="W2" r:id="rId5"/>
+    <hyperlink ref="Q2" r:id="rId1"/>
+    <hyperlink ref="Q3" r:id="rId2"/>
+    <hyperlink ref="W2" r:id="rId3"/>
+    <hyperlink ref="Q4" r:id="rId4"/>
+    <hyperlink ref="Q5" r:id="rId5"/>
+    <hyperlink ref="Q6" r:id="rId6"/>
+    <hyperlink ref="B2" r:id="rId7"/>
+    <hyperlink ref="B3" r:id="rId8"/>
+    <hyperlink ref="Q7" r:id="rId9"/>
+    <hyperlink ref="B7" r:id="rId10"/>
+    <hyperlink ref="B5" r:id="rId11"/>
+    <hyperlink ref="B6" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
cleaning up the way errors are handled and removing extra  file name field
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/demo_mods.xlsx
+++ b/spec/fixtures/files/demo_mods.xlsx
@@ -512,7 +512,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
-    <numFmt numFmtId="166" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -573,7 +573,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -866,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CR7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" zoomScalePageLayoutView="127" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fix for solr title array and changing creator role to be pipe delimited to follow standard
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/demo_mods.xlsx
+++ b/spec/fixtures/files/demo_mods.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="159">
   <si>
     <t>What is your name?</t>
   </si>
@@ -290,9 +290,6 @@
     <t>Series Title</t>
   </si>
   <si>
-    <t>Creator 1 Role Value URI</t>
-  </si>
-  <si>
     <t>Creator 2 Role Value URI</t>
   </si>
   <si>
@@ -504,6 +501,9 @@
   </si>
   <si>
     <t>http://hdl.handle.net/2047/D10000740</t>
+  </si>
+  <si>
+    <t>Creator|http://id.loc.gov/vocabulary/relators/cre</t>
   </si>
 </sst>
 </file>
@@ -864,10 +864,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CR7"/>
+  <dimension ref="A1:CQ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -888,85 +888,84 @@
     <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="51.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="29.1640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="51" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="19" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="9" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="8" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="104.83203125" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="102" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="34" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="45.33203125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="28" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="45.33203125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="28" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="28" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="28" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="28" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="28" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="28" bestFit="1" customWidth="1"/>
-    <col min="83" max="87" width="28" customWidth="1"/>
-    <col min="88" max="88" width="50.5" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="72.5" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="34" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="35.83203125" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="51.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="51" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="19" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="8" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="104.83203125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="102" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="34" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="28" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="28" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="28" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="28" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="28" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="28" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="28" bestFit="1" customWidth="1"/>
+    <col min="82" max="86" width="28" customWidth="1"/>
+    <col min="87" max="87" width="50.5" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="72.5" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="34" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="35.83203125" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1007,7 +1006,7 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>13</v>
@@ -1016,160 +1015,160 @@
         <v>14</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="W1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="X1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="AB1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AI1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="AE1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="AH1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AO1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="AK1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="AP1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AS1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="AQ1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="AT1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="BD1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AU1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="BE1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="BI1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="BF1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="BG1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="BH1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="BI1" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="BJ1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BP1" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="BK1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="BL1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="BM1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BN1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BO1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="BQ1" s="1" t="s">
         <v>95</v>
@@ -1211,7 +1210,7 @@
         <v>107</v>
       </c>
       <c r="CD1" s="1" t="s">
-        <v>108</v>
+        <v>147</v>
       </c>
       <c r="CE1" s="1" t="s">
         <v>148</v>
@@ -1223,7 +1222,7 @@
         <v>150</v>
       </c>
       <c r="CH1" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="CI1" s="1" t="s">
         <v>154</v>
@@ -1235,36 +1234,33 @@
         <v>156</v>
       </c>
       <c r="CL1" s="1" t="s">
-        <v>157</v>
+        <v>84</v>
       </c>
       <c r="CM1" s="1" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="CN1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="CO1" s="1" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="CP1" s="1" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="CQ1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="CR1" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>60</v>
@@ -1286,42 +1282,40 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>66</v>
       </c>
       <c r="P2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="U2" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="Q2" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="R2" s="1"/>
-      <c r="S2" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="U2" s="6" t="s">
+      <c r="V2" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="W2" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="V2" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="X2" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="Y2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
@@ -1339,70 +1333,72 @@
       <c r="AN2" s="1"/>
       <c r="AO2" s="1"/>
       <c r="AP2" s="1"/>
-      <c r="AQ2" s="1"/>
+      <c r="AQ2" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="AR2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AS2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AS2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AT2" s="1">
+        <v>1981</v>
+      </c>
+      <c r="AU2" s="1">
+        <v>1982</v>
+      </c>
+      <c r="AV2" s="1"/>
+      <c r="AW2" s="1"/>
+      <c r="AX2" s="1">
+        <v>1982</v>
+      </c>
+      <c r="AY2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AZ2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA2" s="1"/>
+      <c r="BB2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BC2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BD2" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="AU2" s="1">
-        <v>1981</v>
-      </c>
-      <c r="AV2" s="1">
-        <v>1982</v>
-      </c>
-      <c r="AW2" s="1"/>
-      <c r="AX2" s="1"/>
-      <c r="AY2" s="1">
-        <v>1982</v>
-      </c>
-      <c r="AZ2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="BA2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="BB2" s="1"/>
-      <c r="BC2" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="BD2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="BE2" s="7" t="s">
+      <c r="BE2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BF2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BG2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BH2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="BI2" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="BF2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="BG2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="BH2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="BI2" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="BJ2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BK2" s="1"/>
+      <c r="BL2" s="1"/>
+      <c r="BM2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BN2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BO2" s="1"/>
+      <c r="BP2" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="BK2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="BL2" s="1"/>
-      <c r="BM2" s="1"/>
-      <c r="BN2" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="BO2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="BP2" s="1"/>
       <c r="BQ2" s="1" t="s">
         <v>116</v>
       </c>
@@ -1410,126 +1406,121 @@
         <v>117</v>
       </c>
       <c r="BS2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="BT2" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="BT2" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="BU2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="BV2" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="BV2" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="BW2" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="BX2" s="1" t="s">
-        <v>117</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="BX2" s="1"/>
       <c r="BY2" s="1"/>
       <c r="BZ2" s="1"/>
       <c r="CA2" s="1"/>
       <c r="CB2" s="1"/>
       <c r="CC2" s="1"/>
-      <c r="CD2" s="1"/>
+      <c r="CD2" s="1" t="s">
+        <v>134</v>
+      </c>
       <c r="CE2" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="CF2" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="CG2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="CH2" s="1"/>
-      <c r="CI2" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="CJ2" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="CK2" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="CL2" s="2"/>
+      <c r="CG2" s="1"/>
+      <c r="CH2" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="CI2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="CJ2" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="CK2" s="2"/>
+      <c r="CL2" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="CM2" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="CN2" s="1" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="CO2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="CP2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="CQ2" s="3">
+      <c r="CP2" s="3">
         <v>42170.508518518516</v>
       </c>
-      <c r="CR2" s="1" t="s">
+      <c r="CQ2" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>58</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>123</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>124</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>62</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
       <c r="M3" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="O3" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="P3" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q3" s="5" t="s">
+      <c r="P3" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="T3" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="T3" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="U3" s="8" t="s">
-        <v>111</v>
-      </c>
+      <c r="U3" s="8"/>
       <c r="V3" s="8"/>
       <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="6" t="s">
+      <c r="X3" s="6" t="s">
         <v>68</v>
       </c>
+      <c r="Y3" s="8"/>
       <c r="Z3" s="8"/>
       <c r="AA3" s="8"/>
       <c r="AB3" s="8"/>
@@ -1547,187 +1538,184 @@
       <c r="AN3" s="8"/>
       <c r="AO3" s="8"/>
       <c r="AP3" s="8"/>
-      <c r="AQ3" s="8"/>
+      <c r="AQ3" s="6" t="s">
+        <v>69</v>
+      </c>
       <c r="AR3" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="AS3" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="AS3" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="AT3" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="AT3" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="AU3" s="6" t="s">
+      <c r="AU3" s="8"/>
+      <c r="AV3" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="AV3" s="8"/>
-      <c r="AW3" s="6" t="s">
-        <v>128</v>
-      </c>
+      <c r="AW3" s="8"/>
       <c r="AX3" s="8"/>
-      <c r="AY3" s="8"/>
+      <c r="AY3" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="AZ3" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="BA3" s="6" t="s">
         <v>71</v>
       </c>
+      <c r="BA3" s="8"/>
       <c r="BB3" s="8"/>
       <c r="BC3" s="8"/>
       <c r="BD3" s="8"/>
-      <c r="BE3" s="8"/>
+      <c r="BE3" s="6" t="s">
+        <v>74</v>
+      </c>
       <c r="BF3" s="6" t="s">
-        <v>74</v>
+        <v>128</v>
       </c>
       <c r="BG3" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="BH3" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="BI3" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="BJ3" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="BH3" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="BI3" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="BJ3" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="BK3" s="6" t="s">
+      <c r="BK3" s="8"/>
+      <c r="BL3" s="8"/>
+      <c r="BM3" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="BN3" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="BO3" s="8"/>
+      <c r="BP3" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="BQ3" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="BR3" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="BL3" s="8"/>
-      <c r="BM3" s="8"/>
-      <c r="BN3" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="BO3" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="BP3" s="8"/>
-      <c r="BQ3" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="BR3" s="6" t="s">
-        <v>117</v>
-      </c>
       <c r="BS3" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="BT3" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="BU3" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="BV3" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="BT3" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="BU3" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="BV3" s="6" t="s">
-        <v>117</v>
-      </c>
       <c r="BW3" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="BX3" s="6" t="s">
-        <v>117</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="BX3" s="6"/>
       <c r="BY3" s="6"/>
       <c r="BZ3" s="6"/>
       <c r="CA3" s="6"/>
       <c r="CB3" s="6"/>
       <c r="CC3" s="6"/>
-      <c r="CD3" s="6"/>
-      <c r="CE3" s="6" t="s">
+      <c r="CD3" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="CE3" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="CF3" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="CG3" s="6"/>
+      <c r="CH3" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="CF3" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="CG3" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="CH3" s="6"/>
-      <c r="CI3" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="CJ3" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="CK3" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="CL3" s="9"/>
+      <c r="CI3" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="CJ3" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="CK3" s="9"/>
+      <c r="CL3" s="6" t="s">
+        <v>124</v>
+      </c>
       <c r="CM3" s="6" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="CN3" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="CO3" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="CP3" s="10">
+        <v>42243.733247824071</v>
+      </c>
+      <c r="CQ3" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="CO3" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="CP3" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="CQ3" s="10">
-        <v>42243.733247824071</v>
-      </c>
-      <c r="CR3" s="6" t="s">
-        <v>134</v>
-      </c>
     </row>
-    <row r="4" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>58</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>123</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>124</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>62</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
       <c r="M4" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="O4" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="P4" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q4" s="5" t="s">
+      <c r="P4" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="T4" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="T4" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="U4" s="8" t="s">
-        <v>111</v>
-      </c>
+      <c r="U4" s="8"/>
       <c r="V4" s="8"/>
       <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="6" t="s">
+      <c r="X4" s="6" t="s">
         <v>68</v>
       </c>
+      <c r="Y4" s="8"/>
       <c r="Z4" s="8"/>
       <c r="AA4" s="8"/>
       <c r="AB4" s="8"/>
@@ -1745,146 +1733,145 @@
       <c r="AN4" s="8"/>
       <c r="AO4" s="8"/>
       <c r="AP4" s="8"/>
-      <c r="AQ4" s="8"/>
+      <c r="AQ4" s="6" t="s">
+        <v>69</v>
+      </c>
       <c r="AR4" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="AS4" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="AS4" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="AT4" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="AT4" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="AU4" s="6" t="s">
+      <c r="AU4" s="8"/>
+      <c r="AV4" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="AV4" s="8"/>
-      <c r="AW4" s="6" t="s">
-        <v>128</v>
-      </c>
+      <c r="AW4" s="8"/>
       <c r="AX4" s="8"/>
-      <c r="AY4" s="8"/>
+      <c r="AY4" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="AZ4" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="BA4" s="6" t="s">
         <v>71</v>
       </c>
+      <c r="BA4" s="8"/>
       <c r="BB4" s="8"/>
       <c r="BC4" s="8"/>
       <c r="BD4" s="8"/>
-      <c r="BE4" s="8"/>
+      <c r="BE4" s="6" t="s">
+        <v>74</v>
+      </c>
       <c r="BF4" s="6" t="s">
-        <v>74</v>
+        <v>128</v>
       </c>
       <c r="BG4" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="BH4" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="BI4" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="BJ4" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="BH4" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="BI4" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="BJ4" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="BK4" s="6" t="s">
+      <c r="BK4" s="8"/>
+      <c r="BL4" s="8"/>
+      <c r="BM4" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="BN4" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="BO4" s="8"/>
+      <c r="BP4" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="BQ4" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="BR4" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="BL4" s="8"/>
-      <c r="BM4" s="8"/>
-      <c r="BN4" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="BO4" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="BP4" s="8"/>
-      <c r="BQ4" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="BR4" s="6" t="s">
-        <v>117</v>
-      </c>
       <c r="BS4" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="BT4" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="BU4" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="BV4" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="BT4" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="BU4" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="BV4" s="6" t="s">
-        <v>117</v>
-      </c>
       <c r="BW4" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="BX4" s="6" t="s">
-        <v>117</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="BX4" s="6"/>
       <c r="BY4" s="6"/>
       <c r="BZ4" s="6"/>
       <c r="CA4" s="6"/>
       <c r="CB4" s="6"/>
       <c r="CC4" s="6"/>
-      <c r="CD4" s="6"/>
-      <c r="CE4" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="CF4" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="CG4" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="CH4" s="6"/>
+      <c r="CD4" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="CE4" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="CF4" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="CG4" s="6"/>
+      <c r="CH4" s="1" t="s">
+        <v>134</v>
+      </c>
       <c r="CI4" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="CJ4" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="CK4" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="CL4" s="9"/>
+      <c r="CK4" s="9"/>
+      <c r="CL4" s="6" t="s">
+        <v>124</v>
+      </c>
       <c r="CM4" s="6" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="CN4" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="CO4" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="CP4" s="10">
+        <v>42243.733247824071</v>
+      </c>
+      <c r="CQ4" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="CO4" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="CP4" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="CQ4" s="10">
-        <v>42243.733247824071</v>
-      </c>
-      <c r="CR4" s="6" t="s">
-        <v>134</v>
-      </c>
     </row>
-    <row r="5" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>58</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>123</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>124</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>62</v>
@@ -1896,36 +1883,34 @@
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
       <c r="M5" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="O5" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="P5" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q5" s="5" t="s">
+      <c r="P5" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="S5" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="T5" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="T5" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="U5" s="8" t="s">
-        <v>111</v>
-      </c>
+      <c r="U5" s="8"/>
       <c r="V5" s="8"/>
       <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="6" t="s">
+      <c r="X5" s="6" t="s">
         <v>68</v>
       </c>
+      <c r="Y5" s="8"/>
       <c r="Z5" s="8"/>
       <c r="AA5" s="8"/>
       <c r="AB5" s="8"/>
@@ -1943,126 +1928,125 @@
       <c r="AN5" s="8"/>
       <c r="AO5" s="8"/>
       <c r="AP5" s="8"/>
-      <c r="AQ5" s="8"/>
+      <c r="AQ5" s="6" t="s">
+        <v>69</v>
+      </c>
       <c r="AR5" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="AS5" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="AS5" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="AT5" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="AT5" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="AU5" s="6" t="s">
+      <c r="AU5" s="8"/>
+      <c r="AV5" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="AV5" s="8"/>
-      <c r="AW5" s="6" t="s">
-        <v>128</v>
-      </c>
+      <c r="AW5" s="8"/>
       <c r="AX5" s="8"/>
-      <c r="AY5" s="8"/>
+      <c r="AY5" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="AZ5" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="BA5" s="6" t="s">
         <v>71</v>
       </c>
+      <c r="BA5" s="8"/>
       <c r="BB5" s="8"/>
       <c r="BC5" s="8"/>
       <c r="BD5" s="8"/>
-      <c r="BE5" s="8"/>
+      <c r="BE5" s="6" t="s">
+        <v>74</v>
+      </c>
       <c r="BF5" s="6" t="s">
-        <v>74</v>
+        <v>128</v>
       </c>
       <c r="BG5" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="BH5" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="BI5" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="BJ5" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="BH5" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="BI5" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="BJ5" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="BK5" s="6" t="s">
+      <c r="BK5" s="8"/>
+      <c r="BL5" s="8"/>
+      <c r="BM5" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="BN5" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="BO5" s="8"/>
+      <c r="BP5" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="BQ5" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="BR5" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="BL5" s="8"/>
-      <c r="BM5" s="8"/>
-      <c r="BN5" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="BO5" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="BP5" s="8"/>
-      <c r="BQ5" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="BR5" s="6" t="s">
-        <v>117</v>
-      </c>
       <c r="BS5" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="BT5" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="BU5" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="BV5" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="BT5" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="BU5" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="BV5" s="6" t="s">
-        <v>117</v>
-      </c>
       <c r="BW5" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="BX5" s="6" t="s">
-        <v>117</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="BX5" s="6"/>
       <c r="BY5" s="6"/>
       <c r="BZ5" s="6"/>
       <c r="CA5" s="6"/>
       <c r="CB5" s="6"/>
       <c r="CC5" s="6"/>
-      <c r="CD5" s="6"/>
-      <c r="CE5" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="CF5" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="CG5" s="6" t="s">
-        <v>111</v>
-      </c>
+      <c r="CD5" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="CE5" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="CF5" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="CG5" s="6"/>
       <c r="CH5" s="6"/>
       <c r="CI5" s="6"/>
-      <c r="CJ5" s="6"/>
-      <c r="CK5" s="8"/>
-      <c r="CL5" s="9"/>
+      <c r="CJ5" s="8"/>
+      <c r="CK5" s="9"/>
+      <c r="CL5" s="6" t="s">
+        <v>124</v>
+      </c>
       <c r="CM5" s="6" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="CN5" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="CO5" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="CP5" s="3">
+        <v>42170.508518518516</v>
+      </c>
+      <c r="CQ5" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="CO5" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="CP5" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="CQ5" s="3">
-        <v>42170.508518518516</v>
-      </c>
-      <c r="CR5" s="6" t="s">
-        <v>134</v>
-      </c>
     </row>
-    <row r="6" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>58</v>
       </c>
@@ -2070,56 +2054,54 @@
         <v>59</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>123</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>124</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>62</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
       <c r="M6" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="O6" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="P6" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q6" s="5" t="s">
+      <c r="P6" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="T6" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="T6" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="U6" s="8" t="s">
-        <v>111</v>
-      </c>
+      <c r="U6" s="8"/>
       <c r="V6" s="8"/>
       <c r="W6" s="8"/>
-      <c r="X6" s="8"/>
-      <c r="Y6" s="6" t="s">
+      <c r="X6" s="6" t="s">
         <v>68</v>
       </c>
+      <c r="Y6" s="8"/>
       <c r="Z6" s="8"/>
       <c r="AA6" s="8"/>
       <c r="AB6" s="8"/>
@@ -2137,62 +2119,62 @@
       <c r="AN6" s="8"/>
       <c r="AO6" s="8"/>
       <c r="AP6" s="8"/>
-      <c r="AQ6" s="8"/>
+      <c r="AQ6" s="6" t="s">
+        <v>69</v>
+      </c>
       <c r="AR6" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="AS6" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="AS6" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="AT6" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="AT6" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="AU6" s="6" t="s">
+      <c r="AU6" s="8"/>
+      <c r="AV6" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="AV6" s="8"/>
-      <c r="AW6" s="6" t="s">
-        <v>128</v>
-      </c>
+      <c r="AW6" s="8"/>
       <c r="AX6" s="8"/>
-      <c r="AY6" s="8"/>
+      <c r="AY6" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="AZ6" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="BA6" s="6" t="s">
         <v>71</v>
       </c>
+      <c r="BA6" s="8"/>
       <c r="BB6" s="8"/>
       <c r="BC6" s="8"/>
       <c r="BD6" s="8"/>
-      <c r="BE6" s="8"/>
+      <c r="BE6" s="6" t="s">
+        <v>74</v>
+      </c>
       <c r="BF6" s="6" t="s">
-        <v>74</v>
+        <v>128</v>
       </c>
       <c r="BG6" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="BH6" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="BI6" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="BJ6" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="BH6" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="BI6" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="BJ6" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="BK6" s="6" t="s">
-        <v>130</v>
-      </c>
+      <c r="BK6" s="8"/>
       <c r="BL6" s="8"/>
-      <c r="BM6" s="8"/>
+      <c r="BM6" s="6" t="s">
+        <v>79</v>
+      </c>
       <c r="BN6" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="BO6" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="BP6" s="8"/>
+      <c r="BO6" s="8"/>
+      <c r="BP6" s="6"/>
       <c r="BQ6" s="6"/>
       <c r="BR6" s="6"/>
       <c r="BS6" s="6"/>
@@ -2212,86 +2194,83 @@
       <c r="CG6" s="6"/>
       <c r="CH6" s="6"/>
       <c r="CI6" s="6"/>
-      <c r="CJ6" s="6"/>
-      <c r="CK6" s="8"/>
-      <c r="CL6" s="9"/>
+      <c r="CJ6" s="8"/>
+      <c r="CK6" s="9"/>
+      <c r="CL6" s="6" t="s">
+        <v>124</v>
+      </c>
       <c r="CM6" s="6" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="CN6" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="CO6" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="CP6" s="11">
+        <v>42243.733247824071</v>
+      </c>
+      <c r="CQ6" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="CO6" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="CP6" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="CQ6" s="11">
-        <v>42243.733247824071</v>
-      </c>
-      <c r="CR6" s="6" t="s">
-        <v>134</v>
-      </c>
     </row>
-    <row r="7" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>58</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>123</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>124</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>62</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
       <c r="M7" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="O7" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="P7" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q7" s="5" t="s">
+      <c r="P7" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="T7" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="T7" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="U7" s="8" t="s">
-        <v>111</v>
-      </c>
+      <c r="U7" s="8"/>
       <c r="V7" s="8"/>
       <c r="W7" s="8"/>
-      <c r="X7" s="8"/>
-      <c r="Y7" s="6" t="s">
+      <c r="X7" s="6" t="s">
         <v>68</v>
       </c>
+      <c r="Y7" s="8"/>
       <c r="Z7" s="8"/>
       <c r="AA7" s="8"/>
       <c r="AB7" s="8"/>
@@ -2309,68 +2288,68 @@
       <c r="AN7" s="8"/>
       <c r="AO7" s="8"/>
       <c r="AP7" s="8"/>
-      <c r="AQ7" s="8"/>
+      <c r="AQ7" s="6" t="s">
+        <v>69</v>
+      </c>
       <c r="AR7" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="AS7" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="AS7" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="AT7" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="AT7" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="AU7" s="6" t="s">
+      <c r="AU7" s="8"/>
+      <c r="AV7" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="AV7" s="8"/>
-      <c r="AW7" s="6" t="s">
-        <v>128</v>
-      </c>
+      <c r="AW7" s="8"/>
       <c r="AX7" s="8"/>
-      <c r="AY7" s="8"/>
+      <c r="AY7" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="AZ7" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="BA7" s="6" t="s">
         <v>71</v>
       </c>
+      <c r="BA7" s="8"/>
       <c r="BB7" s="8"/>
       <c r="BC7" s="8"/>
       <c r="BD7" s="8"/>
-      <c r="BE7" s="8"/>
+      <c r="BE7" s="6" t="s">
+        <v>74</v>
+      </c>
       <c r="BF7" s="6" t="s">
-        <v>74</v>
+        <v>128</v>
       </c>
       <c r="BG7" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="BH7" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="BI7" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="BJ7" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="BH7" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="BI7" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="BJ7" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="BK7" s="6" t="s">
-        <v>130</v>
-      </c>
+      <c r="BK7" s="8"/>
       <c r="BL7" s="8"/>
-      <c r="BM7" s="8"/>
+      <c r="BM7" s="6" t="s">
+        <v>79</v>
+      </c>
       <c r="BN7" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="BO7" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="BP7" s="8"/>
+      <c r="BO7" s="8"/>
+      <c r="BP7" s="6" t="s">
+        <v>117</v>
+      </c>
       <c r="BQ7" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="BR7" s="6" t="s">
-        <v>117</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="BR7" s="6"/>
       <c r="BS7" s="6"/>
       <c r="BT7" s="6"/>
       <c r="BU7" s="6"/>
@@ -2388,47 +2367,40 @@
       <c r="CG7" s="6"/>
       <c r="CH7" s="6"/>
       <c r="CI7" s="6"/>
-      <c r="CJ7" s="6"/>
-      <c r="CK7" s="8"/>
-      <c r="CL7" s="9"/>
+      <c r="CJ7" s="8"/>
+      <c r="CK7" s="9"/>
+      <c r="CL7" s="6" t="s">
+        <v>124</v>
+      </c>
       <c r="CM7" s="6" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="CN7" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="CO7" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="CP7" s="11">
+        <v>42243.733247824071</v>
+      </c>
+      <c r="CQ7" s="6" t="s">
         <v>133</v>
-      </c>
-      <c r="CO7" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="CP7" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="CQ7" s="11">
-        <v>42243.733247824071</v>
-      </c>
-      <c r="CR7" s="6" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="BN2">
+  <conditionalFormatting sqref="BM2">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(BN2))&gt;0</formula>
+      <formula>LEN(TRIM(BM2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="Q2" r:id="rId1"/>
-    <hyperlink ref="Q3" r:id="rId2"/>
-    <hyperlink ref="W2" r:id="rId3"/>
-    <hyperlink ref="Q4" r:id="rId4"/>
-    <hyperlink ref="Q5" r:id="rId5"/>
-    <hyperlink ref="Q6" r:id="rId6"/>
-    <hyperlink ref="B2" r:id="rId7"/>
-    <hyperlink ref="B3" r:id="rId8"/>
-    <hyperlink ref="Q7" r:id="rId9"/>
-    <hyperlink ref="B7" r:id="rId10"/>
-    <hyperlink ref="B5" r:id="rId11"/>
-    <hyperlink ref="B6" r:id="rId12"/>
+    <hyperlink ref="V2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="B7" r:id="rId4"/>
+    <hyperlink ref="B5" r:id="rId5"/>
+    <hyperlink ref="B6" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
adding some spec tests for the loader - focusing on new files and mods for now
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/demo_mods.xlsx
+++ b/spec/fixtures/files/demo_mods.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="161">
   <si>
     <t>What is your name?</t>
   </si>
@@ -504,6 +504,12 @@
   </si>
   <si>
     <t>Creator|http://id.loc.gov/vocabulary/relators/cre</t>
+  </si>
+  <si>
+    <t>supplied</t>
+  </si>
+  <si>
+    <t>affiliated</t>
   </si>
 </sst>
 </file>
@@ -866,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CQ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1269,7 +1275,7 @@
         <v>61</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>62</v>
+        <v>159</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>63</v>
@@ -1293,7 +1299,9 @@
       <c r="P2" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="Q2" s="1"/>
+      <c r="Q2" s="1" t="s">
+        <v>160</v>
+      </c>
       <c r="R2" s="6" t="s">
         <v>138</v>
       </c>

</xml_diff>

<commit_message>
updating spec fixtures for new language format
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/demo_mods.xlsx
+++ b/spec/fixtures/files/demo_mods.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27211"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="159">
   <si>
     <t>What is your name?</t>
   </si>
@@ -173,9 +173,6 @@
     <t>Digital Origin</t>
   </si>
   <si>
-    <t>Language</t>
-  </si>
-  <si>
     <t>Abstract</t>
   </si>
   <si>
@@ -260,9 +257,6 @@
     <t>reformatted digital</t>
   </si>
   <si>
-    <t>English</t>
-  </si>
-  <si>
     <t>Annual report from the Citywide Educational Coalition includes seminal information about the desegregation of the Boston Public Schools.</t>
   </si>
   <si>
@@ -308,9 +302,6 @@
     <t>Frequency Authority</t>
   </si>
   <si>
-    <t>Language URI</t>
-  </si>
-  <si>
     <t>Topical Subject Heading 1</t>
   </si>
   <si>
@@ -371,9 +362,6 @@
     <t>marcfrequency</t>
   </si>
   <si>
-    <t>http://id.loc.gov/vocabulary/iso639-2/eng</t>
-  </si>
-  <si>
     <t>African American students -- Massachusetts -- Boston</t>
   </si>
   <si>
@@ -510,6 +498,12 @@
   </si>
   <si>
     <t>affiliated</t>
+  </si>
+  <si>
+    <t>Language 1</t>
+  </si>
+  <si>
+    <t>English | http://id.loc.gov/vocabulary/iso639-2/eng</t>
   </si>
 </sst>
 </file>
@@ -870,10 +864,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CQ7"/>
+  <dimension ref="A1:CP7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" topLeftCell="AZ1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="BH1" sqref="BH1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -938,40 +932,39 @@
     <col min="58" max="58" width="8" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="104.83203125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="102" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="34" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="45.33203125" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="28" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="45.33203125" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="28" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="28" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="28" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="28" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="28" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="28" bestFit="1" customWidth="1"/>
-    <col min="82" max="86" width="28" customWidth="1"/>
-    <col min="87" max="87" width="50.5" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="72.5" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="34" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="35.83203125" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="104.83203125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="102" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="34" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="28" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="28" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="28" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="28" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="28" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="28" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="28" bestFit="1" customWidth="1"/>
+    <col min="81" max="85" width="28" customWidth="1"/>
+    <col min="86" max="86" width="50.5" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="72.5" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="34" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="35.83203125" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:95" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1012,7 +1005,7 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>13</v>
@@ -1027,7 +1020,7 @@
         <v>16</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>17</v>
@@ -1036,7 +1029,7 @@
         <v>18</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>19</v>
@@ -1048,7 +1041,7 @@
         <v>21</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>22</v>
@@ -1057,7 +1050,7 @@
         <v>23</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AD1" s="1" t="s">
         <v>24</v>
@@ -1066,7 +1059,7 @@
         <v>25</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="AG1" s="1" t="s">
         <v>26</v>
@@ -1075,7 +1068,7 @@
         <v>27</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AJ1" s="1" t="s">
         <v>28</v>
@@ -1084,7 +1077,7 @@
         <v>29</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="AM1" s="1" t="s">
         <v>30</v>
@@ -1093,7 +1086,7 @@
         <v>31</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AP1" s="1" t="s">
         <v>32</v>
@@ -1105,7 +1098,7 @@
         <v>34</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AT1" s="1" t="s">
         <v>35</v>
@@ -1138,7 +1131,7 @@
         <v>44</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="BE1" s="1" t="s">
         <v>45</v>
@@ -1150,10 +1143,10 @@
         <v>47</v>
       </c>
       <c r="BH1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="BI1" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="BI1" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="BJ1" s="1" t="s">
         <v>49</v>
@@ -1171,157 +1164,154 @@
         <v>53</v>
       </c>
       <c r="BO1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="BY1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="CA1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="CB1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="CC1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="CD1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="CE1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="CF1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="CG1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="CH1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="CI1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="CJ1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="CK1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="CL1" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="BQ1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="BR1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="BS1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="BT1" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="BU1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="BV1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="BW1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="BX1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="BY1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="BZ1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="CA1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="CB1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="CC1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="CD1" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="CE1" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="CF1" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="CG1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="CH1" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="CI1" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="CJ1" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="CK1" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="CL1" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="CM1" s="1" t="s">
         <v>55</v>
       </c>
       <c r="CN1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="CO1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="CO1" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="CP1" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:94" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="CQ1" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:95" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="B2" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="R2" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="O2" s="1" t="s">
+      <c r="S2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="U2" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="U2" s="6" t="s">
+      <c r="V2" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="V2" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="W2" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
@@ -1342,13 +1332,13 @@
       <c r="AO2" s="1"/>
       <c r="AP2" s="1"/>
       <c r="AQ2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AR2" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="AS2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="AT2" s="1">
         <v>1981</v>
@@ -1362,171 +1352,168 @@
         <v>1982</v>
       </c>
       <c r="AY2" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AZ2" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="BA2" s="1"/>
       <c r="BB2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BC2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="BC2" s="1" t="s">
+      <c r="BD2" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="BE2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="BD2" s="7" t="s">
+      <c r="BF2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BG2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BH2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="BI2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BJ2" s="1"/>
+      <c r="BK2" s="1"/>
+      <c r="BL2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="BM2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BN2" s="1"/>
+      <c r="BO2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="BP2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="BQ2" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="BE2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="BF2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="BG2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="BH2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="BI2" s="1" t="s">
+      <c r="BR2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="BS2" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="BJ2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="BK2" s="1"/>
-      <c r="BL2" s="1"/>
-      <c r="BM2" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="BN2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="BO2" s="1"/>
-      <c r="BP2" s="1" t="s">
+      <c r="BT2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="BU2" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="BQ2" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="BR2" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="BS2" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="BT2" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="BU2" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="BV2" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="BW2" s="1" t="s">
-        <v>116</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="BW2" s="1"/>
       <c r="BX2" s="1"/>
       <c r="BY2" s="1"/>
       <c r="BZ2" s="1"/>
       <c r="CA2" s="1"/>
       <c r="CB2" s="1"/>
-      <c r="CC2" s="1"/>
+      <c r="CC2" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="CD2" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="CE2" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="CF2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="CG2" s="1"/>
-      <c r="CH2" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="CI2" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="CJ2" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="CK2" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="CF2" s="1"/>
+      <c r="CG2" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="CH2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="CI2" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="CJ2" s="2"/>
+      <c r="CK2" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="CL2" s="1" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="CM2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="CN2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="CO2" s="3">
+        <v>42170.508518518516</v>
+      </c>
+      <c r="CP2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="CN2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:94" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="CO2" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="CP2" s="3">
-        <v>42170.508518518516</v>
-      </c>
-      <c r="CQ2" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:95" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>62</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="6" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
       <c r="M3" s="6" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="Q3" s="8"/>
       <c r="R3" s="8" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="S3" s="6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="U3" s="8"/>
       <c r="V3" s="8"/>
       <c r="W3" s="8"/>
       <c r="X3" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Y3" s="8"/>
       <c r="Z3" s="8"/>
@@ -1547,181 +1534,178 @@
       <c r="AO3" s="8"/>
       <c r="AP3" s="8"/>
       <c r="AQ3" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AR3" s="6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="AS3" s="9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="AT3" s="6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="AU3" s="8"/>
       <c r="AV3" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="AW3" s="8"/>
       <c r="AX3" s="8"/>
       <c r="AY3" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AZ3" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="BA3" s="8"/>
       <c r="BB3" s="8"/>
       <c r="BC3" s="8"/>
       <c r="BD3" s="8"/>
       <c r="BE3" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="BF3" s="6" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="BG3" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="BH3" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="BH3" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="BI3" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="BJ3" s="8"/>
+      <c r="BK3" s="8"/>
+      <c r="BL3" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="BI3" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="BJ3" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="BK3" s="8"/>
-      <c r="BL3" s="8"/>
       <c r="BM3" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="BN3" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="BO3" s="8"/>
+        <v>78</v>
+      </c>
+      <c r="BN3" s="8"/>
+      <c r="BO3" s="6" t="s">
+        <v>113</v>
+      </c>
       <c r="BP3" s="6" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="BQ3" s="6" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="BR3" s="6" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="BS3" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BT3" s="6" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="BU3" s="6" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="BV3" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="BW3" s="6" t="s">
-        <v>116</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="BW3" s="6"/>
       <c r="BX3" s="6"/>
       <c r="BY3" s="6"/>
       <c r="BZ3" s="6"/>
       <c r="CA3" s="6"/>
       <c r="CB3" s="6"/>
-      <c r="CC3" s="6"/>
-      <c r="CD3" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="CE3" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="CF3" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="CG3" s="6"/>
-      <c r="CH3" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="CI3" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="CJ3" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="CK3" s="9"/>
+      <c r="CC3" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="CD3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="CE3" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="CF3" s="6"/>
+      <c r="CG3" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="CH3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="CI3" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="CJ3" s="9"/>
+      <c r="CK3" s="6" t="s">
+        <v>120</v>
+      </c>
       <c r="CL3" s="6" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="CM3" s="6" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="CN3" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="CO3" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="CP3" s="10">
+        <v>80</v>
+      </c>
+      <c r="CO3" s="10">
         <v>42243.733247824071</v>
       </c>
-      <c r="CQ3" s="6" t="s">
-        <v>133</v>
+      <c r="CP3" s="6" t="s">
+        <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:95" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="8" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="6" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
       <c r="M4" s="6" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="Q4" s="8"/>
       <c r="R4" s="8" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="S4" s="6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="U4" s="8"/>
       <c r="V4" s="8"/>
       <c r="W4" s="8"/>
       <c r="X4" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Y4" s="8"/>
       <c r="Z4" s="8"/>
@@ -1742,147 +1726,144 @@
       <c r="AO4" s="8"/>
       <c r="AP4" s="8"/>
       <c r="AQ4" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AR4" s="6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="AS4" s="9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="AT4" s="6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="AU4" s="8"/>
       <c r="AV4" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="AW4" s="8"/>
       <c r="AX4" s="8"/>
       <c r="AY4" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AZ4" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="BA4" s="8"/>
       <c r="BB4" s="8"/>
       <c r="BC4" s="8"/>
       <c r="BD4" s="8"/>
       <c r="BE4" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="BF4" s="6" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="BG4" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="BH4" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="BH4" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="BI4" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="BJ4" s="8"/>
+      <c r="BK4" s="8"/>
+      <c r="BL4" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="BI4" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="BJ4" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="BK4" s="8"/>
-      <c r="BL4" s="8"/>
       <c r="BM4" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="BN4" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="BO4" s="8"/>
+        <v>78</v>
+      </c>
+      <c r="BN4" s="8"/>
+      <c r="BO4" s="6" t="s">
+        <v>113</v>
+      </c>
       <c r="BP4" s="6" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="BQ4" s="6" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="BR4" s="6" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="BS4" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BT4" s="6" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="BU4" s="6" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="BV4" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="BW4" s="6" t="s">
-        <v>116</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="BW4" s="6"/>
       <c r="BX4" s="6"/>
       <c r="BY4" s="6"/>
       <c r="BZ4" s="6"/>
       <c r="CA4" s="6"/>
       <c r="CB4" s="6"/>
-      <c r="CC4" s="6"/>
-      <c r="CD4" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="CE4" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="CF4" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="CG4" s="6"/>
+      <c r="CC4" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="CD4" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="CE4" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="CF4" s="6"/>
+      <c r="CG4" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="CH4" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="CI4" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="CJ4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="CK4" s="9"/>
+        <v>65</v>
+      </c>
+      <c r="CJ4" s="9"/>
+      <c r="CK4" s="6" t="s">
+        <v>120</v>
+      </c>
       <c r="CL4" s="6" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="CM4" s="6" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="CN4" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="CO4" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="CP4" s="10">
+        <v>80</v>
+      </c>
+      <c r="CO4" s="10">
         <v>42243.733247824071</v>
       </c>
-      <c r="CQ4" s="6" t="s">
-        <v>133</v>
+      <c r="CP4" s="6" t="s">
+        <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:95" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="6"/>
@@ -1891,32 +1872,32 @@
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
       <c r="M5" s="6" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="Q5" s="8"/>
       <c r="R5" s="8" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="S5" s="6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="T5" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="U5" s="8"/>
       <c r="V5" s="8"/>
       <c r="W5" s="8"/>
       <c r="X5" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Y5" s="8"/>
       <c r="Z5" s="8"/>
@@ -1937,177 +1918,174 @@
       <c r="AO5" s="8"/>
       <c r="AP5" s="8"/>
       <c r="AQ5" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AR5" s="6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="AS5" s="9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="AT5" s="6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="AU5" s="8"/>
       <c r="AV5" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="AW5" s="8"/>
       <c r="AX5" s="8"/>
       <c r="AY5" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AZ5" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="BA5" s="8"/>
       <c r="BB5" s="8"/>
       <c r="BC5" s="8"/>
       <c r="BD5" s="8"/>
       <c r="BE5" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="BF5" s="6" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="BG5" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="BH5" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="BH5" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="BI5" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="BJ5" s="8"/>
+      <c r="BK5" s="8"/>
+      <c r="BL5" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="BI5" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="BJ5" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="BK5" s="8"/>
-      <c r="BL5" s="8"/>
       <c r="BM5" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="BN5" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="BO5" s="8"/>
+        <v>78</v>
+      </c>
+      <c r="BN5" s="8"/>
+      <c r="BO5" s="6" t="s">
+        <v>113</v>
+      </c>
       <c r="BP5" s="6" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="BQ5" s="6" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="BR5" s="6" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="BS5" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BT5" s="6" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="BU5" s="6" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="BV5" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="BW5" s="6" t="s">
-        <v>116</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="BW5" s="6"/>
       <c r="BX5" s="6"/>
       <c r="BY5" s="6"/>
       <c r="BZ5" s="6"/>
       <c r="CA5" s="6"/>
       <c r="CB5" s="6"/>
-      <c r="CC5" s="6"/>
-      <c r="CD5" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="CE5" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="CF5" s="6" t="s">
-        <v>110</v>
-      </c>
+      <c r="CC5" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="CD5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="CE5" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="CF5" s="6"/>
       <c r="CG5" s="6"/>
       <c r="CH5" s="6"/>
-      <c r="CI5" s="6"/>
-      <c r="CJ5" s="8"/>
-      <c r="CK5" s="9"/>
+      <c r="CI5" s="8"/>
+      <c r="CJ5" s="9"/>
+      <c r="CK5" s="6" t="s">
+        <v>120</v>
+      </c>
       <c r="CL5" s="6" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="CM5" s="6" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="CN5" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="CO5" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="CP5" s="3">
+        <v>80</v>
+      </c>
+      <c r="CO5" s="3">
         <v>42170.508518518516</v>
       </c>
-      <c r="CQ5" s="6" t="s">
-        <v>133</v>
+      <c r="CP5" s="6" t="s">
+        <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:95" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="C6" s="8" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="6" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
       <c r="M6" s="6" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="Q6" s="8"/>
       <c r="R6" s="8" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="T6" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="U6" s="8"/>
       <c r="V6" s="8"/>
       <c r="W6" s="8"/>
       <c r="X6" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Y6" s="8"/>
       <c r="Z6" s="8"/>
@@ -2128,60 +2106,58 @@
       <c r="AO6" s="8"/>
       <c r="AP6" s="8"/>
       <c r="AQ6" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AR6" s="6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="AS6" s="9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="AT6" s="6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="AU6" s="8"/>
       <c r="AV6" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="AW6" s="8"/>
       <c r="AX6" s="8"/>
       <c r="AY6" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AZ6" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="BA6" s="8"/>
       <c r="BB6" s="8"/>
       <c r="BC6" s="8"/>
       <c r="BD6" s="8"/>
       <c r="BE6" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="BF6" s="6" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="BG6" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="BH6" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="BH6" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="BI6" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="BJ6" s="8"/>
+      <c r="BK6" s="8"/>
+      <c r="BL6" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="BI6" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="BJ6" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="BK6" s="8"/>
-      <c r="BL6" s="8"/>
       <c r="BM6" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="BN6" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="BO6" s="8"/>
+        <v>78</v>
+      </c>
+      <c r="BN6" s="8"/>
+      <c r="BO6" s="6"/>
       <c r="BP6" s="6"/>
       <c r="BQ6" s="6"/>
       <c r="BR6" s="6"/>
@@ -2201,82 +2177,81 @@
       <c r="CF6" s="6"/>
       <c r="CG6" s="6"/>
       <c r="CH6" s="6"/>
-      <c r="CI6" s="6"/>
-      <c r="CJ6" s="8"/>
-      <c r="CK6" s="9"/>
+      <c r="CI6" s="8"/>
+      <c r="CJ6" s="9"/>
+      <c r="CK6" s="6" t="s">
+        <v>120</v>
+      </c>
       <c r="CL6" s="6" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="CM6" s="6" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="CN6" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="CO6" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="CP6" s="11">
+        <v>80</v>
+      </c>
+      <c r="CO6" s="11">
         <v>42243.733247824071</v>
       </c>
-      <c r="CQ6" s="6" t="s">
-        <v>133</v>
+      <c r="CP6" s="6" t="s">
+        <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:95" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="6" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
       <c r="M7" s="6" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="Q7" s="8"/>
       <c r="R7" s="8" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="S7" s="6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="T7" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="U7" s="8"/>
       <c r="V7" s="8"/>
       <c r="W7" s="8"/>
       <c r="X7" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Y7" s="8"/>
       <c r="Z7" s="8"/>
@@ -2297,66 +2272,64 @@
       <c r="AO7" s="8"/>
       <c r="AP7" s="8"/>
       <c r="AQ7" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AR7" s="6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="AS7" s="9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="AT7" s="6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="AU7" s="8"/>
       <c r="AV7" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="AW7" s="8"/>
       <c r="AX7" s="8"/>
       <c r="AY7" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AZ7" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="BA7" s="8"/>
       <c r="BB7" s="8"/>
       <c r="BC7" s="8"/>
       <c r="BD7" s="8"/>
       <c r="BE7" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="BF7" s="6" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="BG7" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="BH7" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="BH7" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="BI7" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="BJ7" s="8"/>
+      <c r="BK7" s="8"/>
+      <c r="BL7" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="BI7" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="BJ7" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="BK7" s="8"/>
-      <c r="BL7" s="8"/>
       <c r="BM7" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="BN7" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="BO7" s="8"/>
+        <v>78</v>
+      </c>
+      <c r="BN7" s="8"/>
+      <c r="BO7" s="6" t="s">
+        <v>113</v>
+      </c>
       <c r="BP7" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="BQ7" s="6" t="s">
-        <v>116</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="BQ7" s="6"/>
       <c r="BR7" s="6"/>
       <c r="BS7" s="6"/>
       <c r="BT7" s="6"/>
@@ -2374,32 +2347,31 @@
       <c r="CF7" s="6"/>
       <c r="CG7" s="6"/>
       <c r="CH7" s="6"/>
-      <c r="CI7" s="6"/>
-      <c r="CJ7" s="8"/>
-      <c r="CK7" s="9"/>
+      <c r="CI7" s="8"/>
+      <c r="CJ7" s="9"/>
+      <c r="CK7" s="6" t="s">
+        <v>120</v>
+      </c>
       <c r="CL7" s="6" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="CM7" s="6" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="CN7" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="CO7" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="CP7" s="11">
+        <v>80</v>
+      </c>
+      <c r="CO7" s="11">
         <v>42243.733247824071</v>
       </c>
-      <c r="CQ7" s="6" t="s">
-        <v>133</v>
+      <c r="CP7" s="6" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="BM2">
+  <conditionalFormatting sqref="BL2">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(BM2))&gt;0</formula>
+      <formula>LEN(TRIM(BL2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>